<commit_message>
chore: sync all local changes
</commit_message>
<xml_diff>
--- a/export/UBER_Investment_Report.xlsx
+++ b/export/UBER_Investment_Report.xlsx
@@ -10,6 +10,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Decision_Card" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Curated_Evidence" sheetId="2" state="visible" r:id="rId2"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Metric_Cheat_Sheet" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Key_Inputs_Human" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -134,23 +135,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="CuratedEvidence" displayName="CuratedEvidence" ref="A1:F13" headerRowCount="1">
-  <autoFilter ref="A1:F13"/>
-  <tableColumns count="6">
-    <tableColumn id="1" name="published_at"/>
-    <tableColumn id="2" name="risk_tag"/>
-    <tableColumn id="3" name="impact_score"/>
-    <tableColumn id="4" name="source"/>
-    <tableColumn id="5" name="title"/>
-    <tableColumn id="6" name="url"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium9" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="MetricCheatSheet" displayName="MetricCheatSheet" ref="A1:F7" headerRowCount="1">
-  <autoFilter ref="A1:F7"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TMetricCheatSheet" displayName="TMetricCheatSheet" ref="A1:F8" headerRowCount="1">
+  <autoFilter ref="A1:F8"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Metric"/>
     <tableColumn id="2" name="Meaning"/>
@@ -452,7 +438,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -497,7 +483,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2026-02-18 20:05 UTC</t>
+          <t>2026-02-19 03:11 UTC</t>
         </is>
       </c>
     </row>
@@ -508,7 +494,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>83</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5">
@@ -519,7 +505,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>AVOID</t>
         </is>
       </c>
     </row>
@@ -529,9 +515,6 @@
           <t>data_completeness_score</t>
         </is>
       </c>
-      <c r="B6" t="n">
-        <v>100</v>
-      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -539,43 +522,52 @@
           <t>confidence_score</t>
         </is>
       </c>
-      <c r="B7" t="n">
-        <v>39</v>
-      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>bucket_scores</t>
+          <t>confidence_explainer</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>{"cash_level": 21, "valuation": 15, "growth": 16, "quality": 15, "balance_risk": 16}</t>
+          <t>Higher = easier to verify sources quickly. Low = concentrated sources / fewer top-tier links.</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>lights</t>
+          <t>bucket_scores</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>{"cash_level": "GREEN", "valuation": "YELLOW", "growth": "YELLOW", "quality": "YELLOW", "balance_risk": "YELLOW"}</t>
+          <t>{"cash_level": 21, "valuation": 17, "growth": 0, "quality": 6, "balance_risk": 8}</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
+          <t>lights</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>{"cash_level": "GREEN", "valuation": "YELLOW", "growth": "YELLOW", "quality": "YELLOW", "balance_risk": "YELLOW"}</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
           <t>red_flags</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>["[MED] Free cash flow is volatile", "[MED] Repeated negative risk theme: TOTAL"]</t>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>["TTM revenue declining YoY", "TTM FCF declining YoY", "Net debt high vs TTM FCF", "Frequent LABOR/INSURANCE/REGULATORY negatives (30d)"]</t>
         </is>
       </c>
     </row>
@@ -590,420 +582,23 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="22" customWidth="1" min="1" max="1"/>
-    <col width="12" customWidth="1" min="2" max="2"/>
-    <col width="14" customWidth="1" min="3" max="3"/>
-    <col width="12" customWidth="1" min="4" max="4"/>
-    <col width="60" customWidth="1" min="5" max="5"/>
-    <col width="60" customWidth="1" min="6" max="6"/>
-  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="inlineStr">
-        <is>
-          <t>published_at</t>
-        </is>
-      </c>
-      <c r="B1" s="2" t="inlineStr">
-        <is>
-          <t>risk_tag</t>
-        </is>
-      </c>
-      <c r="C1" s="2" t="inlineStr">
-        <is>
-          <t>impact_score</t>
-        </is>
-      </c>
-      <c r="D1" s="2" t="inlineStr">
-        <is>
-          <t>source</t>
-        </is>
-      </c>
-      <c r="E1" s="2" t="inlineStr">
-        <is>
-          <t>title</t>
-        </is>
-      </c>
-      <c r="F1" s="2" t="inlineStr">
-        <is>
-          <t>url</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>2026-02-18 19:08 UTC</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>OTHER</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>finnhub</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Uber offers incentives for EV chargers, Wendy's stock surges</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>https://finnhub.io/api/news?id=8ccbcd773be9ce94b90f1df2a5c8b76d516bbd8b1d5a28c337fbc7c7b01cfffd</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2026-02-18 18:28 UTC</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>OTHER</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>0</v>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>finnhub</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Uber to Invest $100M in Autonomous Vehicle Charging Network</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>https://finnhub.io/api/news?id=5bfba49d337267800a787eb955a182e34544dadc572208cd8823efc22b2d66a1</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>2026-02-18 17:50 UTC</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>OTHER</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>finnhub</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Jim Cramer Discusses “Over Trading” In Uber (UBER) Stock</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>https://finnhub.io/api/news?id=1593168d794381e0ec754a0cb36efdc1ab933442c39023b4537fb8cefc8ca052</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>2026-02-18 10:27 UTC</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>REGULATORY</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>0</v>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>finnhub</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>'Uber to invest over $100 million in autonomous vehicle charging amid robotaxi push' - Reuters</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>https://finnhub.io/api/news?id=ed87ff791d364694af91cccf5fb5e3cde4f7f62d0e14fd11f5146fcd8a5aed7e</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>2026-02-18 17:13 UTC</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>FINANCIAL</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>0</v>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>finnhub</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>DoorDash Earnings Are Today. It’s All About the Outlook.</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>https://finnhub.io/api/news?id=6f40675ef1ebdfd292c457736b6c46f0a30220010a2e0617ffb66156764e71b9</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>2026-02-18 16:38 UTC</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>OTHER</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
-        <v>0</v>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>finnhub</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>Uber bets big on EV charging for both its drivers and future robotaxis</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>https://finnhub.io/api/news?id=3e8bdb13c1f3c6190a1017e343aadd8edeec172fa68744ff4caeb621a2ea0137</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>2026-02-18 16:38 UTC</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>OTHER</t>
-        </is>
-      </c>
-      <c r="C8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>finnhub</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>Uber to invest $100 million in autonomous vehicle charging hubs for robotaxis</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>https://finnhub.io/api/news?id=f01bb90b992bd85c2b48ec70d4b201bb3d3d7b69ed42314504bb7fbfd9dba1e1</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>2026-02-18 12:08 UTC</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>OTHER</t>
-        </is>
-      </c>
-      <c r="C9" t="n">
-        <v>0</v>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>finnhub</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>Uber to invest over $100 million in autonomous vehicle charging amid robotaxi push</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>https://finnhub.io/api/news?id=e294da39d6e8bae5bb454ae8b076a264fa1fa3872f2c6f8067c3200404f258f4</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>2026-02-18 11:48 UTC</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>OTHER</t>
-        </is>
-      </c>
-      <c r="C10" t="n">
-        <v>0</v>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>finnhub</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>From Rides To Robots: Uber's Path Through The AV And AI Era</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>https://finnhub.io/api/news?id=87844dd58650d9821b047bd9181f4a24f0d1ccf267bb16fae392916e6fd98ddb</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>2026-02-17 19:10 UTC</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>INSURANCE</t>
-        </is>
-      </c>
-      <c r="C11" t="n">
-        <v>0</v>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>finnhub</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>Tesla: Time To Ditch The 'Someday Soon' Premium</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>https://finnhub.io/api/news?id=49baeed6953973567a1027b7a623fe040040faf9c95772258209eec5cd3439a6</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>2026-02-18 03:11 UTC</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>OTHER</t>
-        </is>
-      </c>
-      <c r="C12" t="n">
-        <v>0</v>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>finnhub</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>Wall Street Unable To Understand Coinbase? Brian Armstrong Says Crypto Platform Is Also Underestimated: 'The Laggards Are Going To Be Left Behind'</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>https://finnhub.io/api/news?id=f13aaf497acdc83d659414cb2231184873c782d33cfede71be75bd8c9b9c2914</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>2026-02-18 01:30 UTC</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>OTHER</t>
-        </is>
-      </c>
-      <c r="C13" t="n">
-        <v>0</v>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>finnhub</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>The Optimist Fund Q4 2025 Portfolio Review</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>https://finnhub.io/api/news?id=6348d7c30400eeb839e1b20d8b7bb517c989745d42d1e54d8d55b9db3e3daa89</t>
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>No data</t>
         </is>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <tableParts count="1">
-    <tablePart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-  </tableParts>
 </worksheet>
 </file>
 
@@ -1013,7 +608,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1027,7 +622,7 @@
     <col width="21" customWidth="1" min="3" max="3"/>
     <col width="19" customWidth="1" min="4" max="4"/>
     <col width="12" customWidth="1" min="5" max="5"/>
-    <col width="47" customWidth="1" min="6" max="6"/>
+    <col width="51" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1251,6 +846,38 @@
       <c r="F7" t="inlineStr">
         <is>
           <t>Large shocks often reflect real events.</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Confidence (Veracity)</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>How easy it is to verify sources quickly.</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>&gt; 70</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>40–70</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>&lt; 40</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Low confidence = more manual verification needed.</t>
         </is>
       </c>
     </row>
@@ -1260,4 +887,30 @@
     <tablePart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>No data</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>